<commit_message>
Tweaked some notation, ready to submit?
</commit_message>
<xml_diff>
--- a/docs/Examples/YouTube/PetrologCalculations.xlsx
+++ b/docs/Examples/YouTube/PetrologCalculations.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\PySulfSat\PySulfSat_Structure\docs\Examples\Intro_Example_Petrolog_FC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\PySulfSat\PySulfSat_Structure\docs\Examples\YouTube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4E6D5C-1C89-411A-B32C-78D50329F79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2B2AD2-F438-4F82-BA02-CA94788C4DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15510" activeTab="2" xr2:uid="{0529BD8F-C88F-4E4E-8348-A2BAF1D1D7E9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="2" xr2:uid="{0529BD8F-C88F-4E4E-8348-A2BAF1D1D7E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Petrolog_Output_FRAC_Olv" sheetId="4" r:id="rId1"/>
     <sheet name="Petrolog_Output_FRAC_calc_param" sheetId="3" r:id="rId2"/>
     <sheet name="Petrolog_Output_FRAC" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="99">
   <si>
     <t xml:space="preserve"> SiO2_magma</t>
   </si>
@@ -335,12 +335,6 @@
   </si>
   <si>
     <t xml:space="preserve">Olv-Ford83  </t>
-  </si>
-  <si>
-    <t>fo2_calc</t>
-  </si>
-  <si>
-    <t>fo2_e_calc</t>
   </si>
 </sst>
 </file>
@@ -2743,10 +2737,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572120C9-D3FD-4F41-979E-C1B6093D433B}">
-  <dimension ref="A1:BI32"/>
+  <dimension ref="A1:BG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AW1" sqref="AW1"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="BI3" sqref="BI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2759,7 +2753,7 @@
     <col min="60" max="60" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2934,14 +2928,8 @@
       <c r="BF1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>100</v>
-      </c>
     </row>
-    <row r="2" spans="1:61" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>49.901000000000003</v>
       </c>
@@ -3119,16 +3107,8 @@
       <c r="BG2" s="4">
         <v>0.34809027777777773</v>
       </c>
-      <c r="BH2" s="3">
-        <f>10^AW2</f>
-        <v>1.9054607179632456E-8</v>
-      </c>
-      <c r="BI2" s="3">
-        <f>EXP(AW2)</f>
-        <v>4.4386060390287402E-4</v>
-      </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>49.997799999999998</v>
       </c>
@@ -3307,7 +3287,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>50.098199999999999</v>
       </c>
@@ -3486,7 +3466,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>50.200299999999999</v>
       </c>
@@ -3665,7 +3645,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>50.306199999999997</v>
       </c>
@@ -3844,7 +3824,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>50.414000000000001</v>
       </c>
@@ -4023,7 +4003,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>50.526000000000003</v>
       </c>
@@ -4202,7 +4182,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>50.641300000000001</v>
       </c>
@@ -4381,7 +4361,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>50.760100000000001</v>
       </c>
@@ -4560,7 +4540,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>50.883600000000001</v>
       </c>
@@ -4739,7 +4719,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>51.01</v>
       </c>
@@ -4918,7 +4898,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>51.1417</v>
       </c>
@@ -5097,7 +5077,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>51.277900000000002</v>
       </c>
@@ -5276,7 +5256,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>51.418799999999997</v>
       </c>
@@ -5455,7 +5435,7 @@
         <v>0.34809027777777773</v>
       </c>
     </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>51.566299999999998</v>
       </c>

</xml_diff>